<commit_message>
modifico la clase jugada para solucionar el movimiento de la ficha
</commit_message>
<xml_diff>
--- a/JuegosDeDamas/CONVERSION.xlsx
+++ b/JuegosDeDamas/CONVERSION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salvador.Cirino\Desktop\test\Juegos de Damas\juegos_Damas\JuegosDeDamas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95295E9F-BD1A-467E-BC2C-AEC9C44CAEC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B384C7-34EB-412F-8AB0-D2106C48811B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{36059C5C-9F2F-4861-B479-BCB6A3E45DBD}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="B1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update modifico clases varias
solucion comer rojo, comer azul
</commit_message>
<xml_diff>
--- a/JuegosDeDamas/CONVERSION.xlsx
+++ b/JuegosDeDamas/CONVERSION.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salvador.Cirino\Desktop\test\Juegos de Damas\juegos_Damas\JuegosDeDamas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salvador.Cirino\Desktop\juegos_Damas-Desarrollo Dos\juegos_Damas-Desarrollo\JuegosDeDamas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B384C7-34EB-412F-8AB0-D2106C48811B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758C8F49-C720-492F-A536-A4AC0277CF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{36059C5C-9F2F-4861-B479-BCB6A3E45DBD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>A</t>
   </si>
@@ -162,6 +162,156 @@
   </si>
   <si>
     <t>Numero de posiciones X,Y</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>6,6</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>4,0</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>4,6</t>
+  </si>
+  <si>
+    <t>6,0</t>
+  </si>
+  <si>
+    <t>6,2</t>
+  </si>
+  <si>
+    <t>6,4</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>3,7</t>
+  </si>
+  <si>
+    <t>5,1</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>5,7</t>
+  </si>
+  <si>
+    <t>7,1</t>
+  </si>
+  <si>
+    <t>7,3</t>
+  </si>
+  <si>
+    <t>7,5</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>1,7</t>
+  </si>
+  <si>
+    <t>version correcta matriz C#</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>6,1</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>4,3</t>
+  </si>
+  <si>
+    <t>6,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t>7,4</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>6,5</t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>7,6</t>
   </si>
 </sst>
 </file>
@@ -246,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,7 +414,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -285,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -581,22 +737,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC75248-9B9A-4CB1-AFEF-7B1E86EA95BC}">
-  <dimension ref="B1:K36"/>
+  <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -827,13 +983,13 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
@@ -1031,13 +1187,13 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
@@ -1235,16 +1391,238 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <v>6</v>
+      </c>
+      <c r="J38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="7">
+        <v>0</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="7">
+        <v>2</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="7">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="7">
+        <v>4</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="7">
+        <v>5</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="7">
+        <v>6</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="7">
+        <v>7</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>